<commit_message>
senesence 259, fleeting notes, dailylog update and NCEAS
</commit_message>
<xml_diff>
--- a/data/monitoringPhenology/2025-259_Senescence.xlsx
+++ b/data/monitoringPhenology/2025-259_Senescence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/github/fuelinex/data/monitoringPhenology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71762C73-7C76-CB44-8796-EAF2AED12B32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF670BD-87C2-004B-9703-4A46440445B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29400" yWindow="-2480" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45400" yWindow="-1980" windowWidth="29400" windowHeight="17000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="shoot_elongation" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1789" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1791" uniqueCount="468">
   <si>
     <t>tree_ID</t>
   </si>
@@ -1599,7 +1599,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1779,12 +1779,6 @@
         <fgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1949,7 +1943,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -2198,7 +2192,7 @@
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1260360</xdr:colOff>
-      <xdr:row>91</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>10414</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -2312,18 +2306,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{427BC000-52E3-6840-B950-CDCA9CA72D7D}" name="Table1" displayName="Table1" ref="A1:N435" totalsRowShown="0" dataDxfId="13">
-  <autoFilter ref="A1:N435" xr:uid="{427BC000-52E3-6840-B950-CDCA9CA72D7D}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="3">
-      <filters>
-        <filter val="betula"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:N435" xr:uid="{427BC000-52E3-6840-B950-CDCA9CA72D7D}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{0515CFC8-9FED-CA41-BC7E-0EADE3E17C0D}" name="tree_ID" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{C257128B-E55F-4840-ABD4-C2DA6F8965CA}" name="bloc" dataDxfId="11"/>
@@ -2664,9 +2647,9 @@
   <dimension ref="A1:N435"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
       <selection activeCell="A493" sqref="A493"/>
-      <selection pane="topRight" activeCell="L440" sqref="L440"/>
+      <selection pane="topRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2723,7 +2706,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="2" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -2758,7 +2741,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -2793,7 +2776,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -2828,7 +2811,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -2863,7 +2846,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -2898,7 +2881,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -2933,7 +2916,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -2968,7 +2951,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -3003,7 +2986,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -3038,7 +3021,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -3073,7 +3056,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -3108,7 +3091,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -3143,7 +3126,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -3178,7 +3161,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -3213,7 +3196,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -3248,7 +3231,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -3283,7 +3266,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -3318,7 +3301,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -3353,7 +3336,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -3388,7 +3371,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -3423,7 +3406,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -3458,7 +3441,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -3493,7 +3476,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -3528,7 +3511,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -3563,7 +3546,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -3598,7 +3581,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -3633,7 +3616,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -3668,7 +3651,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -3703,7 +3686,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>38</v>
       </c>
@@ -3738,7 +3721,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -3773,7 +3756,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>40</v>
       </c>
@@ -3808,7 +3791,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>42</v>
       </c>
@@ -3843,7 +3826,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>43</v>
       </c>
@@ -3878,7 +3861,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>44</v>
       </c>
@@ -3913,7 +3896,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>45</v>
       </c>
@@ -3948,7 +3931,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>46</v>
       </c>
@@ -3983,7 +3966,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>47</v>
       </c>
@@ -4018,7 +4001,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>48</v>
       </c>
@@ -4053,7 +4036,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>49</v>
       </c>
@@ -4088,7 +4071,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>50</v>
       </c>
@@ -4123,7 +4106,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>51</v>
       </c>
@@ -4158,7 +4141,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>52</v>
       </c>
@@ -4193,7 +4176,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>53</v>
       </c>
@@ -4228,7 +4211,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>54</v>
       </c>
@@ -4263,7 +4246,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>55</v>
       </c>
@@ -4298,7 +4281,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>56</v>
       </c>
@@ -4333,7 +4316,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>58</v>
       </c>
@@ -4368,7 +4351,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>59</v>
       </c>
@@ -4403,7 +4386,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>60</v>
       </c>
@@ -4438,7 +4421,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>61</v>
       </c>
@@ -4473,7 +4456,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>62</v>
       </c>
@@ -4508,7 +4491,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>63</v>
       </c>
@@ -4543,7 +4526,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>64</v>
       </c>
@@ -4578,7 +4561,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>65</v>
       </c>
@@ -4613,7 +4596,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>66</v>
       </c>
@@ -4648,7 +4631,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>67</v>
       </c>
@@ -4683,7 +4666,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>68</v>
       </c>
@@ -4718,7 +4701,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>69</v>
       </c>
@@ -4753,7 +4736,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>70</v>
       </c>
@@ -4788,7 +4771,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>71</v>
       </c>
@@ -4823,7 +4806,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>72</v>
       </c>
@@ -4858,7 +4841,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>74</v>
       </c>
@@ -4893,7 +4876,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="64" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>75</v>
       </c>
@@ -4928,7 +4911,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="65" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>76</v>
       </c>
@@ -4963,7 +4946,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>77</v>
       </c>
@@ -4998,7 +4981,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="67" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>78</v>
       </c>
@@ -5033,7 +5016,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>79</v>
       </c>
@@ -5068,7 +5051,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="69" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>80</v>
       </c>
@@ -5103,7 +5086,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="70" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>81</v>
       </c>
@@ -5138,7 +5121,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>82</v>
       </c>
@@ -5173,7 +5156,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>83</v>
       </c>
@@ -5208,7 +5191,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="73" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>84</v>
       </c>
@@ -5243,7 +5226,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="74" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>85</v>
       </c>
@@ -5278,7 +5261,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="75" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>86</v>
       </c>
@@ -5313,7 +5296,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="76" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>87</v>
       </c>
@@ -5348,7 +5331,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="77" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>88</v>
       </c>
@@ -5383,7 +5366,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="78" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>90</v>
       </c>
@@ -5418,7 +5401,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="79" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>91</v>
       </c>
@@ -5453,7 +5436,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="80" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>92</v>
       </c>
@@ -5488,7 +5471,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="81" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>93</v>
       </c>
@@ -5523,7 +5506,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="82" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>94</v>
       </c>
@@ -5558,7 +5541,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>95</v>
       </c>
@@ -5593,7 +5576,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="84" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>96</v>
       </c>
@@ -5628,7 +5611,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="85" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>97</v>
       </c>
@@ -5663,7 +5646,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="86" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>98</v>
       </c>
@@ -5698,7 +5681,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="87" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>99</v>
       </c>
@@ -5733,7 +5716,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="88" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>100</v>
       </c>
@@ -5768,7 +5751,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="89" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>101</v>
       </c>
@@ -5803,7 +5786,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="90" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>102</v>
       </c>
@@ -5838,7 +5821,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="91" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>103</v>
       </c>
@@ -6048,7 +6031,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="97" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>111</v>
       </c>
@@ -6083,7 +6066,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="98" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>112</v>
       </c>
@@ -6118,7 +6101,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="99" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>113</v>
       </c>
@@ -6153,7 +6136,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="100" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>114</v>
       </c>
@@ -6188,7 +6171,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="101" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>115</v>
       </c>
@@ -6223,7 +6206,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="102" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>116</v>
       </c>
@@ -6258,7 +6241,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="103" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>117</v>
       </c>
@@ -6293,7 +6276,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="104" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>118</v>
       </c>
@@ -6328,7 +6311,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="105" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>119</v>
       </c>
@@ -6363,7 +6346,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="106" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>120</v>
       </c>
@@ -6573,7 +6556,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="112" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>126</v>
       </c>
@@ -6608,7 +6591,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="113" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>127</v>
       </c>
@@ -6643,7 +6626,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="114" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>128</v>
       </c>
@@ -6678,7 +6661,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="115" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>129</v>
       </c>
@@ -6713,7 +6696,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="116" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>130</v>
       </c>
@@ -6748,7 +6731,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="117" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>131</v>
       </c>
@@ -6783,7 +6766,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="118" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>132</v>
       </c>
@@ -6818,7 +6801,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="119" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>133</v>
       </c>
@@ -6853,7 +6836,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="120" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>134</v>
       </c>
@@ -6888,7 +6871,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="121" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>135</v>
       </c>
@@ -7098,7 +7081,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="127" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>141</v>
       </c>
@@ -7133,7 +7116,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="128" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>142</v>
       </c>
@@ -7168,7 +7151,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="129" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>143</v>
       </c>
@@ -7203,7 +7186,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="130" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>144</v>
       </c>
@@ -7238,7 +7221,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="131" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>145</v>
       </c>
@@ -7273,7 +7256,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="132" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>146</v>
       </c>
@@ -7308,7 +7291,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="133" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>147</v>
       </c>
@@ -7343,7 +7326,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="134" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>148</v>
       </c>
@@ -7378,7 +7361,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="135" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>149</v>
       </c>
@@ -7413,7 +7396,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="136" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>150</v>
       </c>
@@ -7619,12 +7602,14 @@
       <c r="J141">
         <v>21.4</v>
       </c>
-      <c r="K141" s="2"/>
+      <c r="K141" s="2">
+        <v>15.9</v>
+      </c>
       <c r="L141">
         <v>80</v>
       </c>
     </row>
-    <row r="142" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>156</v>
       </c>
@@ -7659,7 +7644,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="143" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>157</v>
       </c>
@@ -7694,7 +7679,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="144" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>158</v>
       </c>
@@ -7729,7 +7714,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="145" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>159</v>
       </c>
@@ -7764,7 +7749,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="146" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>160</v>
       </c>
@@ -7799,7 +7784,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="147" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>161</v>
       </c>
@@ -7834,7 +7819,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="148" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>162</v>
       </c>
@@ -7869,7 +7854,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="149" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>163</v>
       </c>
@@ -7904,7 +7889,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="150" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>164</v>
       </c>
@@ -7939,7 +7924,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="151" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>165</v>
       </c>
@@ -8149,7 +8134,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="157" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>171</v>
       </c>
@@ -8184,7 +8169,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="158" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>172</v>
       </c>
@@ -8219,7 +8204,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="159" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>173</v>
       </c>
@@ -8254,7 +8239,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="160" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>174</v>
       </c>
@@ -8289,7 +8274,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="161" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>175</v>
       </c>
@@ -8324,7 +8309,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="162" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>176</v>
       </c>
@@ -8359,7 +8344,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="163" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>177</v>
       </c>
@@ -8394,7 +8379,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="164" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>178</v>
       </c>
@@ -8429,7 +8414,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="165" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>179</v>
       </c>
@@ -8464,7 +8449,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="166" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>180</v>
       </c>
@@ -8674,7 +8659,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="172" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>186</v>
       </c>
@@ -8709,7 +8694,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="173" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>187</v>
       </c>
@@ -8744,7 +8729,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="174" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>188</v>
       </c>
@@ -8779,7 +8764,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="175" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>189</v>
       </c>
@@ -8814,7 +8799,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="176" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>190</v>
       </c>
@@ -8849,7 +8834,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="177" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>191</v>
       </c>
@@ -8884,7 +8869,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="178" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>192</v>
       </c>
@@ -8919,7 +8904,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="179" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>193</v>
       </c>
@@ -8954,7 +8939,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="180" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>194</v>
       </c>
@@ -8989,7 +8974,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="181" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>195</v>
       </c>
@@ -9024,7 +9009,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="182" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>196</v>
       </c>
@@ -9059,7 +9044,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="183" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>199</v>
       </c>
@@ -9094,7 +9079,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="184" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>200</v>
       </c>
@@ -9129,7 +9114,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="185" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>201</v>
       </c>
@@ -9164,7 +9149,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="186" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>202</v>
       </c>
@@ -9199,7 +9184,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="187" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>203</v>
       </c>
@@ -9237,7 +9222,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="188" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>204</v>
       </c>
@@ -9272,7 +9257,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="189" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>205</v>
       </c>
@@ -9307,7 +9292,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="190" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>206</v>
       </c>
@@ -9342,7 +9327,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="191" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>207</v>
       </c>
@@ -9377,7 +9362,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="192" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>208</v>
       </c>
@@ -9412,7 +9397,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="193" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>209</v>
       </c>
@@ -9447,7 +9432,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="194" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>210</v>
       </c>
@@ -9482,7 +9467,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="195" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>211</v>
       </c>
@@ -9517,7 +9502,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="196" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>212</v>
       </c>
@@ -9552,7 +9537,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="197" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>213</v>
       </c>
@@ -9587,7 +9572,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="198" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>214</v>
       </c>
@@ -9622,7 +9607,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="199" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>215</v>
       </c>
@@ -9657,7 +9642,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="200" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>216</v>
       </c>
@@ -9692,7 +9677,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="201" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>217</v>
       </c>
@@ -9727,7 +9712,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="202" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>218</v>
       </c>
@@ -9762,7 +9747,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="203" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>219</v>
       </c>
@@ -9797,7 +9782,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="204" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>220</v>
       </c>
@@ -9832,7 +9817,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="205" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>221</v>
       </c>
@@ -9867,7 +9852,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="206" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>222</v>
       </c>
@@ -9902,7 +9887,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="207" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>223</v>
       </c>
@@ -9937,7 +9922,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="208" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>224</v>
       </c>
@@ -9972,7 +9957,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="209" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>225</v>
       </c>
@@ -10007,7 +9992,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="210" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>226</v>
       </c>
@@ -10042,7 +10027,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="211" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>227</v>
       </c>
@@ -10077,7 +10062,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="212" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>228</v>
       </c>
@@ -10112,7 +10097,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="213" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>229</v>
       </c>
@@ -10147,7 +10132,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="214" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>230</v>
       </c>
@@ -10182,7 +10167,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="215" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>231</v>
       </c>
@@ -10217,7 +10202,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="216" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>232</v>
       </c>
@@ -10252,7 +10237,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="217" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>233</v>
       </c>
@@ -10287,7 +10272,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="218" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>234</v>
       </c>
@@ -10322,7 +10307,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="219" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>235</v>
       </c>
@@ -10357,7 +10342,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="220" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>236</v>
       </c>
@@ -10392,7 +10377,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="221" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>237</v>
       </c>
@@ -10427,7 +10412,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="222" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>238</v>
       </c>
@@ -10462,7 +10447,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="223" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>239</v>
       </c>
@@ -10497,7 +10482,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="224" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>240</v>
       </c>
@@ -10532,7 +10517,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="225" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>241</v>
       </c>
@@ -10567,7 +10552,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="226" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>242</v>
       </c>
@@ -10602,7 +10587,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="227" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>243</v>
       </c>
@@ -10637,7 +10622,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="228" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>244</v>
       </c>
@@ -10672,7 +10657,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="229" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>245</v>
       </c>
@@ -10707,7 +10692,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="230" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>246</v>
       </c>
@@ -10742,7 +10727,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="231" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>247</v>
       </c>
@@ -10777,7 +10762,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="232" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>248</v>
       </c>
@@ -10812,7 +10797,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="233" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>249</v>
       </c>
@@ -10847,7 +10832,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="234" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>250</v>
       </c>
@@ -10882,7 +10867,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="235" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>251</v>
       </c>
@@ -10917,7 +10902,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="236" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>252</v>
       </c>
@@ -10952,7 +10937,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="237" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>253</v>
       </c>
@@ -10987,7 +10972,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="238" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>254</v>
       </c>
@@ -11022,7 +11007,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="239" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>255</v>
       </c>
@@ -11057,7 +11042,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="240" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>256</v>
       </c>
@@ -11092,7 +11077,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="241" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>257</v>
       </c>
@@ -11127,7 +11112,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="242" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>258</v>
       </c>
@@ -11162,7 +11147,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="243" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>259</v>
       </c>
@@ -11197,7 +11182,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="244" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>260</v>
       </c>
@@ -11232,7 +11217,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="245" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>261</v>
       </c>
@@ -11267,7 +11252,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="246" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>262</v>
       </c>
@@ -11302,7 +11287,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="247" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>263</v>
       </c>
@@ -11337,7 +11322,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="248" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>264</v>
       </c>
@@ -11372,7 +11357,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="249" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>265</v>
       </c>
@@ -11407,7 +11392,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="250" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>266</v>
       </c>
@@ -11442,7 +11427,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="251" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>267</v>
       </c>
@@ -11477,7 +11462,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="252" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>268</v>
       </c>
@@ -11512,7 +11497,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="253" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>269</v>
       </c>
@@ -11547,7 +11532,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="254" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>270</v>
       </c>
@@ -11582,7 +11567,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="255" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>271</v>
       </c>
@@ -11617,7 +11602,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="256" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>272</v>
       </c>
@@ -11652,7 +11637,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="257" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>273</v>
       </c>
@@ -11687,7 +11672,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="258" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>274</v>
       </c>
@@ -11722,7 +11707,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="259" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>275</v>
       </c>
@@ -11757,7 +11742,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="260" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>276</v>
       </c>
@@ -11792,7 +11777,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="261" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>277</v>
       </c>
@@ -11827,7 +11812,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="262" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>278</v>
       </c>
@@ -11862,7 +11847,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="263" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>279</v>
       </c>
@@ -11897,7 +11882,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="264" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>280</v>
       </c>
@@ -11932,7 +11917,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="265" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>281</v>
       </c>
@@ -11967,7 +11952,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="266" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>282</v>
       </c>
@@ -12002,7 +11987,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="267" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>283</v>
       </c>
@@ -12037,7 +12022,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="268" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>284</v>
       </c>
@@ -12072,7 +12057,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="269" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>287</v>
       </c>
@@ -12107,7 +12092,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="270" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>288</v>
       </c>
@@ -12142,7 +12127,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="271" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>289</v>
       </c>
@@ -12177,7 +12162,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="272" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>290</v>
       </c>
@@ -12212,7 +12197,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="273" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>291</v>
       </c>
@@ -12247,7 +12232,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="274" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>292</v>
       </c>
@@ -12282,7 +12267,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="275" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>293</v>
       </c>
@@ -12317,7 +12302,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="276" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>294</v>
       </c>
@@ -12352,7 +12337,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="277" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>295</v>
       </c>
@@ -12387,7 +12372,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="278" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>296</v>
       </c>
@@ -12422,7 +12407,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="279" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>297</v>
       </c>
@@ -12457,7 +12442,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="280" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>298</v>
       </c>
@@ -12492,7 +12477,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="281" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>299</v>
       </c>
@@ -12527,7 +12512,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="282" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>300</v>
       </c>
@@ -12562,7 +12547,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="283" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>301</v>
       </c>
@@ -12597,7 +12582,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="284" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>302</v>
       </c>
@@ -12632,7 +12617,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="285" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>303</v>
       </c>
@@ -12667,7 +12652,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="286" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>304</v>
       </c>
@@ -12702,7 +12687,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="287" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>305</v>
       </c>
@@ -12737,7 +12722,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="288" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>306</v>
       </c>
@@ -12772,7 +12757,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="289" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>307</v>
       </c>
@@ -12807,7 +12792,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="290" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>308</v>
       </c>
@@ -12842,7 +12827,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="291" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>309</v>
       </c>
@@ -12877,7 +12862,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="292" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>310</v>
       </c>
@@ -12912,7 +12897,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="293" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>311</v>
       </c>
@@ -12947,7 +12932,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="294" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>312</v>
       </c>
@@ -12982,7 +12967,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="295" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>313</v>
       </c>
@@ -13017,7 +13002,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="296" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>314</v>
       </c>
@@ -13052,7 +13037,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="297" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>315</v>
       </c>
@@ -13087,7 +13072,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="298" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>316</v>
       </c>
@@ -13122,7 +13107,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="299" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>317</v>
       </c>
@@ -13157,7 +13142,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="300" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>318</v>
       </c>
@@ -13192,7 +13177,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="301" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>319</v>
       </c>
@@ -13227,7 +13212,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="302" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>320</v>
       </c>
@@ -13262,7 +13247,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="303" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>321</v>
       </c>
@@ -13297,7 +13282,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="304" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>322</v>
       </c>
@@ -13332,7 +13317,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="305" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>323</v>
       </c>
@@ -13367,7 +13352,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="306" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>324</v>
       </c>
@@ -13402,7 +13387,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="307" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>325</v>
       </c>
@@ -13437,7 +13422,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="308" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>326</v>
       </c>
@@ -13472,7 +13457,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="309" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>327</v>
       </c>
@@ -13503,6 +13488,9 @@
       <c r="K309" t="s">
         <v>464</v>
       </c>
+      <c r="L309" t="s">
+        <v>464</v>
+      </c>
       <c r="M309" t="s">
         <v>464</v>
       </c>
@@ -13510,7 +13498,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="310" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>328</v>
       </c>
@@ -13545,7 +13533,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="311" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>329</v>
       </c>
@@ -13580,7 +13568,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="312" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>330</v>
       </c>
@@ -13615,7 +13603,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="313" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>331</v>
       </c>
@@ -13650,7 +13638,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="314" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>332</v>
       </c>
@@ -13685,7 +13673,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="315" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>333</v>
       </c>
@@ -13720,7 +13708,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="316" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
         <v>334</v>
       </c>
@@ -13755,7 +13743,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="317" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>335</v>
       </c>
@@ -13790,7 +13778,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="318" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
         <v>336</v>
       </c>
@@ -13825,7 +13813,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="319" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
         <v>337</v>
       </c>
@@ -13860,7 +13848,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="320" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
         <v>338</v>
       </c>
@@ -13891,6 +13879,9 @@
       <c r="K320" t="s">
         <v>464</v>
       </c>
+      <c r="L320" t="s">
+        <v>464</v>
+      </c>
       <c r="M320" t="s">
         <v>464</v>
       </c>
@@ -13898,7 +13889,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="321" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>339</v>
       </c>
@@ -13933,7 +13924,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="322" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>340</v>
       </c>
@@ -13968,7 +13959,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="323" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
         <v>341</v>
       </c>
@@ -14003,7 +13994,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="324" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
         <v>342</v>
       </c>
@@ -14038,7 +14029,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="325" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
         <v>343</v>
       </c>
@@ -14073,7 +14064,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="326" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
         <v>344</v>
       </c>
@@ -14108,7 +14099,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="327" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
         <v>345</v>
       </c>
@@ -14143,7 +14134,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="328" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
         <v>346</v>
       </c>
@@ -14178,7 +14169,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="329" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
         <v>347</v>
       </c>
@@ -14213,7 +14204,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="330" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
         <v>348</v>
       </c>
@@ -14248,7 +14239,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="331" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
         <v>349</v>
       </c>
@@ -14283,7 +14274,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="332" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
         <v>350</v>
       </c>
@@ -14318,7 +14309,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="333" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
         <v>351</v>
       </c>
@@ -14353,7 +14344,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="334" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
         <v>352</v>
       </c>
@@ -14391,7 +14382,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="335" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
         <v>353</v>
       </c>
@@ -14426,7 +14417,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="336" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
         <v>354</v>
       </c>
@@ -14457,9 +14448,11 @@
       <c r="K336">
         <v>22.2</v>
       </c>
-      <c r="L336" s="2"/>
-    </row>
-    <row r="337" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L336" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="337" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
         <v>355</v>
       </c>
@@ -14490,11 +14483,11 @@
       <c r="K337">
         <v>34.700000000000003</v>
       </c>
-      <c r="L337">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="338" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L337" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="338" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
         <v>356</v>
       </c>
@@ -14525,9 +14518,11 @@
       <c r="K338">
         <v>23.8</v>
       </c>
-      <c r="L338" s="2"/>
-    </row>
-    <row r="339" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L338" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="339" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
         <v>357</v>
       </c>
@@ -14562,7 +14557,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="340" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
         <v>358</v>
       </c>
@@ -14597,7 +14592,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="341" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
         <v>359</v>
       </c>
@@ -14632,7 +14627,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="342" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
         <v>360</v>
       </c>
@@ -14673,7 +14668,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="343" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
         <v>361</v>
       </c>
@@ -14708,7 +14703,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="344" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
         <v>362</v>
       </c>
@@ -14743,7 +14738,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="345" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A345" t="s">
         <v>363</v>
       </c>
@@ -14778,7 +14773,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="346" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
         <v>364</v>
       </c>
@@ -14816,7 +14811,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="347" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
         <v>365</v>
       </c>
@@ -14854,7 +14849,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="348" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
         <v>366</v>
       </c>
@@ -14889,7 +14884,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="349" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
         <v>369</v>
       </c>
@@ -14924,7 +14919,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="350" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
         <v>370</v>
       </c>
@@ -14965,7 +14960,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="351" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A351" t="s">
         <v>371</v>
       </c>
@@ -15000,7 +14995,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="352" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A352" t="s">
         <v>372</v>
       </c>
@@ -15035,7 +15030,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="353" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A353" t="s">
         <v>373</v>
       </c>
@@ -15070,7 +15065,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="354" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A354" t="s">
         <v>374</v>
       </c>
@@ -15105,7 +15100,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="355" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A355" t="s">
         <v>375</v>
       </c>
@@ -15140,7 +15135,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="356" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A356" t="s">
         <v>376</v>
       </c>
@@ -15175,7 +15170,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="357" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A357" t="s">
         <v>377</v>
       </c>
@@ -15210,7 +15205,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="358" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A358" t="s">
         <v>378</v>
       </c>
@@ -15245,7 +15240,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="359" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A359" t="s">
         <v>379</v>
       </c>
@@ -15280,7 +15275,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="360" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A360" t="s">
         <v>380</v>
       </c>
@@ -15315,7 +15310,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="361" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A361" t="s">
         <v>381</v>
       </c>
@@ -15350,7 +15345,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="362" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A362" t="s">
         <v>382</v>
       </c>
@@ -15385,7 +15380,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="363" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A363" t="s">
         <v>383</v>
       </c>
@@ -15420,7 +15415,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="364" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A364" t="s">
         <v>384</v>
       </c>
@@ -15455,7 +15450,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="365" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A365" t="s">
         <v>385</v>
       </c>
@@ -15490,7 +15485,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="366" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A366" t="s">
         <v>386</v>
       </c>
@@ -15525,7 +15520,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="367" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A367" t="s">
         <v>387</v>
       </c>
@@ -15560,7 +15555,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="368" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A368" t="s">
         <v>388</v>
       </c>
@@ -15595,7 +15590,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="369" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A369" t="s">
         <v>389</v>
       </c>
@@ -15630,7 +15625,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="370" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A370" t="s">
         <v>390</v>
       </c>
@@ -15665,7 +15660,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="371" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A371" t="s">
         <v>391</v>
       </c>
@@ -15700,7 +15695,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="372" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A372" t="s">
         <v>392</v>
       </c>
@@ -15735,7 +15730,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="373" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A373" t="s">
         <v>393</v>
       </c>
@@ -15770,7 +15765,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="374" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A374" t="s">
         <v>394</v>
       </c>
@@ -15805,7 +15800,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="375" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A375" t="s">
         <v>395</v>
       </c>
@@ -15840,7 +15835,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="376" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A376" t="s">
         <v>396</v>
       </c>
@@ -15875,7 +15870,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="377" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A377" t="s">
         <v>397</v>
       </c>
@@ -15910,7 +15905,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="378" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A378" t="s">
         <v>398</v>
       </c>
@@ -15945,7 +15940,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="379" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A379" t="s">
         <v>399</v>
       </c>
@@ -15980,7 +15975,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="380" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A380" t="s">
         <v>400</v>
       </c>
@@ -16015,7 +16010,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="381" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A381" t="s">
         <v>401</v>
       </c>
@@ -16050,7 +16045,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="382" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A382" t="s">
         <v>402</v>
       </c>
@@ -16085,7 +16080,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="383" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A383" t="s">
         <v>403</v>
       </c>
@@ -16120,7 +16115,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="384" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A384" t="s">
         <v>404</v>
       </c>
@@ -16155,7 +16150,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="385" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A385" t="s">
         <v>405</v>
       </c>
@@ -16190,7 +16185,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="386" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A386" t="s">
         <v>406</v>
       </c>
@@ -16225,7 +16220,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="387" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A387" t="s">
         <v>407</v>
       </c>
@@ -16260,7 +16255,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="388" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A388" t="s">
         <v>408</v>
       </c>
@@ -16295,7 +16290,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="389" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A389" t="s">
         <v>409</v>
       </c>
@@ -16330,7 +16325,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="390" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A390" t="s">
         <v>410</v>
       </c>
@@ -16365,7 +16360,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="391" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A391" t="s">
         <v>411</v>
       </c>
@@ -16400,7 +16395,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="392" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A392" t="s">
         <v>412</v>
       </c>
@@ -16435,7 +16430,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="393" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A393" t="s">
         <v>413</v>
       </c>
@@ -16470,7 +16465,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="394" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A394" t="s">
         <v>414</v>
       </c>
@@ -16505,7 +16500,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="395" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A395" t="s">
         <v>415</v>
       </c>
@@ -16540,7 +16535,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="396" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A396" t="s">
         <v>416</v>
       </c>
@@ -16575,7 +16570,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="397" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A397" t="s">
         <v>417</v>
       </c>
@@ -16610,7 +16605,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="398" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A398" t="s">
         <v>418</v>
       </c>
@@ -16645,7 +16640,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="399" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A399" t="s">
         <v>419</v>
       </c>
@@ -16680,7 +16675,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="400" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A400" t="s">
         <v>420</v>
       </c>
@@ -16715,7 +16710,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="401" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A401" t="s">
         <v>421</v>
       </c>
@@ -16750,7 +16745,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="402" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A402" t="s">
         <v>422</v>
       </c>
@@ -16785,7 +16780,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="403" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A403" t="s">
         <v>423</v>
       </c>
@@ -16820,7 +16815,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="404" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A404" t="s">
         <v>424</v>
       </c>
@@ -16855,7 +16850,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="405" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A405" t="s">
         <v>425</v>
       </c>
@@ -16890,7 +16885,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="406" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A406" t="s">
         <v>426</v>
       </c>
@@ -16925,7 +16920,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="407" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A407" t="s">
         <v>427</v>
       </c>
@@ -16960,7 +16955,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="408" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A408" t="s">
         <v>428</v>
       </c>
@@ -16995,7 +16990,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="409" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A409" t="s">
         <v>429</v>
       </c>
@@ -17030,7 +17025,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="410" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A410" t="s">
         <v>430</v>
       </c>
@@ -17065,7 +17060,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="411" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A411" t="s">
         <v>431</v>
       </c>
@@ -17100,7 +17095,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="412" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A412" t="s">
         <v>432</v>
       </c>
@@ -17135,7 +17130,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="413" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A413" t="s">
         <v>433</v>
       </c>
@@ -17170,7 +17165,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="414" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A414" t="s">
         <v>434</v>
       </c>
@@ -17205,7 +17200,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="415" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A415" t="s">
         <v>435</v>
       </c>
@@ -17240,7 +17235,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="416" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A416" t="s">
         <v>436</v>
       </c>
@@ -17275,7 +17270,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="417" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A417" t="s">
         <v>437</v>
       </c>
@@ -17310,7 +17305,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="418" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A418" t="s">
         <v>438</v>
       </c>
@@ -17345,7 +17340,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="419" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A419" t="s">
         <v>439</v>
       </c>
@@ -17380,7 +17375,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="420" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A420" t="s">
         <v>440</v>
       </c>
@@ -17415,7 +17410,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="421" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A421" t="s">
         <v>441</v>
       </c>
@@ -17450,7 +17445,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="422" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A422" t="s">
         <v>442</v>
       </c>
@@ -17485,7 +17480,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="423" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="423" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A423" t="s">
         <v>443</v>
       </c>
@@ -17520,7 +17515,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="424" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="424" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A424" t="s">
         <v>444</v>
       </c>
@@ -17555,7 +17550,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="425" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A425" t="s">
         <v>445</v>
       </c>
@@ -17590,7 +17585,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="426" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="426" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A426" t="s">
         <v>446</v>
       </c>
@@ -17625,7 +17620,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="427" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="427" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A427" t="s">
         <v>447</v>
       </c>
@@ -17660,7 +17655,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="428" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="428" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A428" t="s">
         <v>448</v>
       </c>
@@ -17695,7 +17690,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="429" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="429" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A429" t="s">
         <v>449</v>
       </c>
@@ -17730,7 +17725,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="430" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="430" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A430" t="s">
         <v>450</v>
       </c>
@@ -17765,7 +17760,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="431" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="431" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A431" t="s">
         <v>451</v>
       </c>
@@ -17800,7 +17795,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="432" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="432" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A432" t="s">
         <v>452</v>
       </c>
@@ -17835,7 +17830,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="433" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="433" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A433" t="s">
         <v>453</v>
       </c>
@@ -17870,7 +17865,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="434" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="434" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A434" t="s">
         <v>454</v>
       </c>
@@ -17905,7 +17900,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="435" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="435" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A435" t="s">
         <v>455</v>
       </c>

</xml_diff>